<commit_message>
business exception message in config
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a0ae9b52c8f1be9/Documents/UiPath/CoinMarketCap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{3C4413D3-CC5D-4212-B459-37326D61B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53C2BDAC-A237-4866-BA89-C35963737399}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{3C4413D3-CC5D-4212-B459-37326D61B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66F1C65C-904E-481B-BF08-7D214F5A72CF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A9E6C398-21A1-4078-B1ED-BAE210854D3F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>key</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>mail_body_error</t>
+  </si>
+  <si>
+    <t>coin_be_error</t>
+  </si>
+  <si>
+    <t>We couldn't load: {0}</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C169D36B-EC9A-4CFE-A822-028041E61520}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,6 +559,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{D6937E1E-D4C0-486A-834D-DB71678D10D3}"/>

</xml_diff>

<commit_message>
load number of coins from config
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a0ae9b52c8f1be9/Documents/UiPath/CoinMarketCap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{3C4413D3-CC5D-4212-B459-37326D61B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66F1C65C-904E-481B-BF08-7D214F5A72CF}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{3C4413D3-CC5D-4212-B459-37326D61B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C10DA8D3-F777-4F6E-88D5-D2C6EEBBC1E4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A9E6C398-21A1-4078-B1ED-BAE210854D3F}"/>
+    <workbookView xWindow="5080" yWindow="2590" windowWidth="28800" windowHeight="15370" xr2:uid="{A9E6C398-21A1-4078-B1ED-BAE210854D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>key</t>
   </si>
@@ -102,6 +102,21 @@
   </si>
   <si>
     <t>We couldn't load: {0}</t>
+  </si>
+  <si>
+    <t>remove_column</t>
+  </si>
+  <si>
+    <t>Column-10,Last 7 Days,Column-0,Circulating Supply,Volume(24h)</t>
+  </si>
+  <si>
+    <t>add_column</t>
+  </si>
+  <si>
+    <t>Old Position,PriceChange,BestBuy,BestSell</t>
+  </si>
+  <si>
+    <t>max_coin</t>
   </si>
 </sst>
 </file>
@@ -467,16 +482,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C169D36B-EC9A-4CFE-A822-028041E61520}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.453125" customWidth="1"/>
-    <col min="2" max="2" width="38.1796875" customWidth="1"/>
+    <col min="2" max="2" width="56.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -565,6 +580,30 @@
       </c>
       <c r="B11" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
another exception and a few small changes, idk
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a0ae9b52c8f1be9/Documents/UiPath/CoinMarketCap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{3C4413D3-CC5D-4212-B459-37326D61B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C10DA8D3-F777-4F6E-88D5-D2C6EEBBC1E4}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{3C4413D3-CC5D-4212-B459-37326D61B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FFFDCFB-D4C6-4AE5-9572-0BB641287A81}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="2590" windowWidth="28800" windowHeight="15370" xr2:uid="{A9E6C398-21A1-4078-B1ED-BAE210854D3F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>key</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>max_coin</t>
+  </si>
+  <si>
+    <t>pgdn_amount</t>
+  </si>
+  <si>
+    <t>website_be_error</t>
+  </si>
+  <si>
+    <t>We couldn't load website: {0}</t>
   </si>
 </sst>
 </file>
@@ -482,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C169D36B-EC9A-4CFE-A822-028041E61520}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,6 +615,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{D6937E1E-D4C0-486A-834D-DB71678D10D3}"/>

</xml_diff>